<commit_message>
added new vessel_data and vessel_name
</commit_message>
<xml_diff>
--- a/src/vessel_data.xlsx
+++ b/src/vessel_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X101"/>
+  <dimension ref="A1:X102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7966,90 +7966,42 @@
           <t>Republic of the Marshall Islands</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>9418468</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>82158</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>42965</t>
-        </is>
+      <c r="C101" t="n">
+        <v>9418468</v>
+      </c>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="n">
+        <v>82158</v>
+      </c>
+      <c r="F101" t="n">
+        <v>42965</v>
       </c>
       <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>94590</t>
-        </is>
-      </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>228.99</t>
-        </is>
-      </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>5649</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="N101" t="inlineStr">
-        <is>
-          <t>222.54</t>
-        </is>
-      </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>14.434</t>
-        </is>
-      </c>
-      <c r="P101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="Q101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="H101" t="n">
+        <v>94590</v>
+      </c>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="n">
+        <v>228.99</v>
+      </c>
+      <c r="K101" t="n">
+        <v>5649</v>
+      </c>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="n">
+        <v>222.54</v>
+      </c>
+      <c r="O101" t="n">
+        <v>14.434</v>
+      </c>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr"/>
       <c r="R101" t="n">
         <v>3</v>
       </c>
-      <c r="S101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="S101" t="inlineStr"/>
+      <c r="T101" t="inlineStr"/>
       <c r="U101" t="inlineStr"/>
       <c r="V101" t="inlineStr">
         <is>
@@ -8057,9 +8009,115 @@
         </is>
       </c>
       <c r="W101" t="inlineStr"/>
-      <c r="X101" t="inlineStr">
-        <is>
-          <t>9710</t>
+      <c r="X101" t="n">
+        <v>9710</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>MP ULTRAMAX 1</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Republic of Singapore</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>9703590</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>63339.85</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>36286</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>75196.6</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>14.4</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>199.9</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>5228</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>194.5</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>11.3</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>13.3</t>
+        </is>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R102" t="n">
+        <v>3</v>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>720</t>
+        </is>
+      </c>
+      <c r="T102" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U102" t="inlineStr"/>
+      <c r="V102" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>